<commit_message>
Some fix in the balance analysis of JPADCore_v2.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/IRON/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/IRON/BALANCE/Balance.xlsx
@@ -247,7 +247,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>2.988345337198654</v>
+        <v>8.545043666543112</v>
       </c>
     </row>
     <row r="5">
@@ -258,7 +258,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>10.414384253628999</v>
+        <v>27.50726038674152</v>
       </c>
     </row>
     <row r="6">
@@ -269,7 +269,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>3.5127680625532145</v>
+        <v>7.545759053209421</v>
       </c>
     </row>
     <row r="7">
@@ -280,7 +280,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>12.027553109411077</v>
+        <v>24.433376021409586</v>
       </c>
     </row>
     <row r="8">
@@ -291,7 +291,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>4.128730561237026</v>
+        <v>7.347756617256282</v>
       </c>
     </row>
     <row r="9">
@@ -302,7 +302,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>13.92230608476055</v>
+        <v>23.824303707023063</v>
       </c>
     </row>
     <row r="10">
@@ -1306,7 +1306,7 @@
         <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>2.1854999999999993</v>
+        <v>33.40549999999999</v>
       </c>
     </row>
     <row r="14">
@@ -1328,7 +1328,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0</v>
+        <v>4.437499999999999</v>
       </c>
     </row>
     <row r="16">
@@ -1350,7 +1350,7 @@
         <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0</v>
+        <v>1.6499999999999997</v>
       </c>
     </row>
     <row r="18">
@@ -1382,7 +1382,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>2.1854999999999993</v>
+        <v>33.40549999999999</v>
       </c>
     </row>
     <row r="22">
@@ -1404,7 +1404,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0</v>
+        <v>-4.437499999999999</v>
       </c>
     </row>
     <row r="24">
@@ -1426,7 +1426,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0</v>
+        <v>1.6499999999999997</v>
       </c>
     </row>
     <row r="26">

</xml_diff>

<commit_message>
More work and some fix in weight and balance analysis.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/IRON/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/IRON/BALANCE/Balance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="37">
   <si>
     <t>Description</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Xcg operating empty mass (max for)</t>
   </si>
   <si>
-    <t>Percent Error</t>
-  </si>
-  <si>
     <t>Xcg LRF</t>
   </si>
   <si>
@@ -102,25 +99,19 @@
     <t>TORENBEEK_1982</t>
   </si>
   <si>
+    <t>Ycg LRF (semi-wing)</t>
+  </si>
+  <si>
+    <t>Ycg BRF (semi-wing)</t>
+  </si>
+  <si>
     <t>Ycg ESTIMATION METHOD COMPARISON</t>
   </si>
   <si>
-    <t>Total Xcg LRF</t>
-  </si>
-  <si>
-    <t>Total Xcg BRF</t>
-  </si>
-  <si>
-    <t>Total Ycg LRF</t>
-  </si>
-  <si>
-    <t>Total Ycg BRF</t>
-  </si>
-  <si>
-    <t>Total Zcg LRF</t>
-  </si>
-  <si>
-    <t>Total Zcg BRF</t>
+    <t>Ycg LRF (semi-tail)</t>
+  </si>
+  <si>
+    <t>Ycg BRF (semi-tail)</t>
   </si>
   <si>
     <t>BALANCE ESTIMATION FOR EACH NACELLE</t>
@@ -225,7 +216,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>6.225057056820859</v>
+        <v>6.284048793214055</v>
       </c>
     </row>
     <row r="3">
@@ -236,105 +227,125 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>20.370784479628455</v>
+        <v>20.552248072446005</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
-        <v>8.545043666543112</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>27.50726038674152</v>
+        <v>8.580362802713651</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>7.545759053209421</v>
+        <v>27.61590505015674</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="n">
-        <v>24.433376021409586</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>7.347756617256282</v>
+        <v>7.5501369346243</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>23.824303707023063</v>
+        <v>24.44684275656683</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>17.702119114986044</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>19.66902123887338</v>
+        <v>7.411821054936215</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>24.02137135995246</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>17.702119114986044</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="n">
+        <v>19.66902123887338</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="n">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="n">
         <v>21.63592336276072</v>
       </c>
     </row>
@@ -361,13 +372,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -378,7 +386,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -389,7 +397,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -400,29 +408,23 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>15.52460075556141</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>15.52460075556141</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -433,31 +435,28 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>15.524600755561412</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-9.308325998589693</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -465,8 +464,16 @@
       <c r="C11" t="n">
         <v>15.524600755561412</v>
       </c>
-      <c r="D11" t="n">
-        <v>-9.308325998589693</v>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>15.524600755561412</v>
       </c>
     </row>
   </sheetData>
@@ -492,13 +499,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -509,7 +513,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -520,7 +524,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -531,111 +535,104 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>21.065548943013923</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>6.183898882356096</v>
+        <v>21.065548943013923</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.3199999999999998</v>
+        <v>6.183898882356096</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-1.3199999999999998</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>2.148114097087354</v>
-      </c>
-      <c r="D10" t="n">
-        <v>19.872438453535377</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>2.1829837889405006</v>
-      </c>
-      <c r="D11" t="n">
-        <v>21.818291793554735</v>
+        <v>2.148114097087354</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2.1829837889405006</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
-        <v>18.465500883744475</v>
-      </c>
-      <c r="D14" t="n">
-        <v>161.2803601846801</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="n">
+        <v>18.465500883744475</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="n">
         <v>6.183898882356097</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-12.500000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -661,13 +658,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -678,7 +672,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -689,7 +683,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -700,83 +694,82 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>33.21353974342176</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>1.7278324361680608</v>
+        <v>33.21353974342176</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1.3399999999999999</v>
+        <v>1.7278324361680608</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.3399999999999999</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1.6735397434217631</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-4.9125145783089</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.6735397434217631</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
         <v>1.727832436168061</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-5.00000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -802,35 +795,32 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>3.7740879999999972</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0981999999999998</v>
+        <v>2.1963999999999997</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -841,83 +831,82 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>31.539999999999996</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>1.0981999999999996</v>
+        <v>35.31408799999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1.4999999999999998</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.1963999999999992</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="n">
-        <v>2.972743999999998</v>
-      </c>
-      <c r="D10" t="n">
-        <v>43.7497098646034</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3.7740879999999972</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1.0981999999999998</v>
-      </c>
-      <c r="D13" t="n">
-        <v>-4.9999999999999885</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2.1963999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -946,51 +935,33 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>1.7483999999999997</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1001,7 +972,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1017,104 +988,104 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>32.96839999999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4.437499999999999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.6499999999999997</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1.7483999999999997</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="n">
-        <v>32.96839999999999</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>4.437499999999999</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0</v>
+        <v>1.7483999999999997</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>1.6499999999999997</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>1.7483999999999997</v>
+        <v>32.96839999999999</v>
       </c>
     </row>
     <row r="21">
@@ -1125,55 +1096,32 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>32.96839999999999</v>
+        <v>-4.437499999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0</v>
+        <v>1.6499999999999997</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="n">
-        <v>-4.437499999999999</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1.6499999999999997</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1203,51 +1151,33 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>2.1854999999999993</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -1258,7 +1188,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1274,104 +1204,104 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>33.40549999999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4.437499999999999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.6499999999999997</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="n">
-        <v>2.1854999999999993</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="n">
-        <v>33.40549999999999</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="n">
-        <v>4.437499999999999</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0</v>
+        <v>2.1854999999999993</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>1.6499999999999997</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>2.1854999999999993</v>
+        <v>33.40549999999999</v>
       </c>
     </row>
     <row r="21">
@@ -1382,55 +1312,32 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>33.40549999999999</v>
+        <v>-4.437499999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0</v>
+        <v>1.6499999999999997</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="n">
-        <v>-4.437499999999999</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1.6499999999999997</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1460,7 +1367,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1471,13 +1378,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>22.349999999999998</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -1493,13 +1400,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -1510,18 +1411,34 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>22.349999999999998</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
         <v>-2.7799999999999994</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on JPADCore_v2 concerning the balance analysis and the LSAerodynamicsCalculator.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/IRON/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/IRON/BALANCE/Balance.xlsx
@@ -229,7 +229,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>6.137611022719621</v>
+        <v>6.158193778588456</v>
       </c>
     </row>
     <row r="3">
@@ -240,7 +240,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>20.101793049712064</v>
+        <v>20.16510735538278</v>
       </c>
     </row>
     <row r="4">
@@ -251,7 +251,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.7605267757572038</v>
+        <v>-0.7604140070405252</v>
       </c>
     </row>
     <row r="5">
@@ -267,7 +267,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>8.303995077089098</v>
+        <v>8.31420991993544</v>
       </c>
     </row>
     <row r="7">
@@ -278,7 +278,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>26.765774447179098</v>
+        <v>26.797196171581454</v>
       </c>
     </row>
     <row r="8">
@@ -289,7 +289,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.44693409599587774</v>
+        <v>0.44695802546495533</v>
       </c>
     </row>
     <row r="9">
@@ -305,7 +305,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>8.303995077089098</v>
+        <v>8.31420991993544</v>
       </c>
     </row>
     <row r="11">
@@ -316,7 +316,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>26.765774447179098</v>
+        <v>26.797196171581454</v>
       </c>
     </row>
     <row r="12">
@@ -327,7 +327,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0.44693409599587774</v>
+        <v>0.44695802546495533</v>
       </c>
     </row>
     <row r="13">
@@ -343,7 +343,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>7.268706588449116</v>
+        <v>7.2761566832357</v>
       </c>
     </row>
     <row r="15">
@@ -354,7 +354,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>23.58113910267801</v>
+        <v>23.604056227168023</v>
       </c>
     </row>
     <row r="16">
@@ -365,7 +365,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.32179798988851327</v>
+        <v>0.3218170343653928</v>
       </c>
     </row>
     <row r="17">
@@ -381,7 +381,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>7.186296489581906</v>
+        <v>7.205145092317862</v>
       </c>
     </row>
     <row r="19">
@@ -392,7 +392,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>23.327638637371848</v>
+        <v>23.385618540679992</v>
       </c>
     </row>
     <row r="20">
@@ -403,7 +403,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.01733077744615341</v>
+        <v>-0.017311574674248202</v>
       </c>
     </row>
     <row r="21">
@@ -608,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>21.065548943013923</v>
+        <v>21.255548943013924</v>
       </c>
     </row>
     <row r="7">
@@ -767,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="n">
-        <v>21.2523759476907</v>
+        <v>21.442375947690707</v>
       </c>
     </row>
     <row r="7">
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>18.012676100376424</v>
+        <v>18.012890076310185</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
More work on ACPerformanceCalculator concerning the take-off analysis.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/IRON/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/IRON/BALANCE/Balance.xlsx
@@ -229,7 +229,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>6.158193778588456</v>
+        <v>6.158017520515703</v>
       </c>
     </row>
     <row r="3">
@@ -240,7 +240,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>20.16510735538278</v>
+        <v>20.1645651705769</v>
       </c>
     </row>
     <row r="4">
@@ -251,7 +251,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.7604140070405252</v>
+        <v>-0.7602401392431766</v>
       </c>
     </row>
     <row r="5">
@@ -267,7 +267,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>8.31420991993544</v>
+        <v>8.314456254821266</v>
       </c>
     </row>
     <row r="7">
@@ -278,7 +278,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>26.797196171581454</v>
+        <v>26.797953918617765</v>
       </c>
     </row>
     <row r="8">
@@ -289,7 +289,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.44695802546495533</v>
+        <v>0.4472319936310508</v>
       </c>
     </row>
     <row r="9">
@@ -305,7 +305,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>8.31420991993544</v>
+        <v>8.314456254821266</v>
       </c>
     </row>
     <row r="11">
@@ -316,7 +316,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>26.797196171581454</v>
+        <v>26.797953918617765</v>
       </c>
     </row>
     <row r="12">
@@ -327,7 +327,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>0.44695802546495533</v>
+        <v>0.4472319936310508</v>
       </c>
     </row>
     <row r="13">
@@ -343,7 +343,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>7.2761566832357</v>
+        <v>7.276247913447818</v>
       </c>
     </row>
     <row r="15">
@@ -354,7 +354,7 @@
         <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>23.604056227168023</v>
+        <v>23.604336859051003</v>
       </c>
     </row>
     <row r="16">
@@ -365,7 +365,7 @@
         <v>6</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3218170343653928</v>
+        <v>0.3220037878413117</v>
       </c>
     </row>
     <row r="17">
@@ -381,7 +381,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>7.205145092317862</v>
+        <v>7.205183127640187</v>
       </c>
     </row>
     <row r="19">
@@ -392,7 +392,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="n">
-        <v>23.385618540679992</v>
+        <v>23.385735540562777</v>
       </c>
     </row>
     <row r="20">
@@ -403,7 +403,7 @@
         <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.017311574674248202</v>
+        <v>-0.017184658529341576</v>
       </c>
     </row>
     <row r="21">
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>18.012890076310185</v>
+        <v>18.011743779366896</v>
       </c>
     </row>
     <row r="3">

</xml_diff>